<commit_message>
rearange data folder and code for traditional augmentation
</commit_message>
<xml_diff>
--- a/ACL_Experiments_Condensed.xlsx
+++ b/ACL_Experiments_Condensed.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Mi unidad\UNAM\2024-II\ACL_classification\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B22FA448-62E9-4136-A4F8-17743B6217D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:20001_{549E9758-3EEC-4D2C-9F55-B99DD89C3564}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{415BAF28-95F9-4C41-A778-60E4FFD128E1}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="84">
   <si>
     <t>Experiment</t>
   </si>
@@ -264,13 +265,37 @@
   </si>
   <si>
     <t>Same as previous experiment, but without cutting the texts to the keyword-phrases</t>
+  </si>
+  <si>
+    <t>Augmentation with paraphrasing, traditional augmentation BUT max_length=128</t>
+  </si>
+  <si>
+    <t>Augmentation with paraphrasing and max_length=256 BUT no traditional augmentation</t>
+  </si>
+  <si>
+    <t>(796, 464, 530, 415)</t>
+  </si>
+  <si>
+    <t>(1000, 580, 1000, 415)</t>
+  </si>
+  <si>
+    <t>(1000, 928, 1000, 747)</t>
+  </si>
+  <si>
+    <t>(2000, 928, 1590, 747)</t>
+  </si>
+  <si>
+    <t>True (1, 2, 3)</t>
+  </si>
+  <si>
+    <t>Augmentation with paraphrasing, traditional augmentation (only for class 1 and 3) and max_length=256</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -324,8 +349,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="16">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -416,6 +448,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="5">
     <border>
@@ -484,7 +522,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
@@ -492,24 +530,6 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -533,10 +553,10 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -551,28 +571,36 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
     <cellStyle name="Überschrift 4" xfId="1" builtinId="19"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor theme="0" tint="-0.14996795556505021"/>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
@@ -911,13 +939,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAFE4854-670F-4ACD-BE38-AF2D488545BF}">
   <dimension ref="A1:X39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" topLeftCell="F11" workbookViewId="0">
+      <selection activeCell="O22" sqref="O22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.5546875" style="20"/>
+    <col min="1" max="1" width="11.5546875" style="14"/>
     <col min="2" max="6" width="11.5546875" style="2"/>
     <col min="7" max="12" width="11.5546875" style="3"/>
     <col min="13" max="15" width="11.5546875" style="4"/>
@@ -926,116 +954,116 @@
     <col min="25" max="16384" width="11.5546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="13" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:24" s="7" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="9" t="s">
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="10" t="s">
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="34"/>
+      <c r="L1" s="34"/>
+      <c r="M1" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="10"/>
-      <c r="O1" s="10"/>
-      <c r="P1" s="11" t="s">
+      <c r="N1" s="35"/>
+      <c r="O1" s="35"/>
+      <c r="P1" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="Q1" s="12" t="s">
+      <c r="Q1" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="R1" s="12"/>
-      <c r="S1" s="12"/>
-      <c r="T1" s="12"/>
-      <c r="U1" s="12"/>
-      <c r="V1" s="12"/>
-      <c r="W1" s="12"/>
-      <c r="X1" s="12"/>
-    </row>
-    <row r="2" spans="1:24" s="13" customFormat="1" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="7"/>
-      <c r="B2" s="14" t="s">
+      <c r="R1" s="32"/>
+      <c r="S1" s="32"/>
+      <c r="T1" s="32"/>
+      <c r="U1" s="32"/>
+      <c r="V1" s="32"/>
+      <c r="W1" s="32"/>
+      <c r="X1" s="32"/>
+    </row>
+    <row r="2" spans="1:24" s="7" customFormat="1" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="30"/>
+      <c r="B2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="15" t="s">
+      <c r="F2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="16" t="s">
+      <c r="G2" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="H2" s="16" t="s">
+      <c r="H2" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="16" t="s">
+      <c r="I2" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="16" t="s">
+      <c r="J2" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="16" t="s">
+      <c r="K2" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="16" t="s">
+      <c r="L2" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="M2" s="17" t="s">
+      <c r="M2" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="N2" s="17" t="s">
+      <c r="N2" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="O2" s="17" t="s">
+      <c r="O2" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="P2" s="11"/>
-      <c r="Q2" s="18" t="s">
+      <c r="P2" s="31"/>
+      <c r="Q2" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="R2" s="18" t="s">
+      <c r="R2" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="S2" s="19" t="s">
+      <c r="S2" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="T2" s="18" t="s">
+      <c r="T2" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="U2" s="18" t="s">
+      <c r="U2" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="V2" s="18" t="s">
+      <c r="V2" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="W2" s="19" t="s">
+      <c r="W2" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="X2" s="19" t="s">
+      <c r="X2" s="13" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A3" s="20">
+      <c r="A3" s="14">
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -1071,7 +1099,7 @@
       <c r="L3" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="M3" s="21">
+      <c r="M3" s="15">
         <v>5.0000000000000002E-5</v>
       </c>
       <c r="N3" s="4">
@@ -1088,13 +1116,13 @@
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A4" s="20">
+      <c r="A4" s="14">
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="23" t="s">
+      <c r="C4" s="17" t="s">
         <v>30</v>
       </c>
       <c r="D4" s="2" t="s">
@@ -1106,7 +1134,7 @@
       <c r="F4" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G4" s="24" t="s">
+      <c r="G4" s="18" t="s">
         <v>31</v>
       </c>
       <c r="H4" s="3" t="s">
@@ -1121,10 +1149,10 @@
       <c r="K4" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="L4" s="24" t="s">
+      <c r="L4" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="M4" s="21">
+      <c r="M4" s="15">
         <v>5.0000000000000002E-5</v>
       </c>
       <c r="N4" s="4">
@@ -1141,16 +1169,16 @@
       </c>
     </row>
     <row r="5" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="20">
+      <c r="A5" s="14">
         <v>3</v>
       </c>
-      <c r="B5" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="C5" s="25" t="s">
+      <c r="B5" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="23" t="s">
+      <c r="D5" s="17" t="s">
         <v>32</v>
       </c>
       <c r="E5" s="2" t="s">
@@ -1159,7 +1187,7 @@
       <c r="F5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G5" s="24" t="s">
+      <c r="G5" s="18" t="s">
         <v>31</v>
       </c>
       <c r="H5" s="3" t="s">
@@ -1174,10 +1202,10 @@
       <c r="K5" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="L5" s="24" t="s">
+      <c r="L5" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="M5" s="21">
+      <c r="M5" s="15">
         <v>6.0000000000000002E-5</v>
       </c>
       <c r="N5" s="4">
@@ -1194,16 +1222,16 @@
       </c>
     </row>
     <row r="6" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="20">
+      <c r="A6" s="14">
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C6" s="25" t="s">
+      <c r="C6" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="25" t="s">
+      <c r="D6" s="19" t="s">
         <v>32</v>
       </c>
       <c r="E6" s="2" t="s">
@@ -1212,7 +1240,7 @@
       <c r="F6" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G6" s="24" t="s">
+      <c r="G6" s="18" t="s">
         <v>31</v>
       </c>
       <c r="H6" s="3" t="s">
@@ -1227,10 +1255,10 @@
       <c r="K6" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="L6" s="24" t="s">
+      <c r="L6" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="M6" s="21">
+      <c r="M6" s="15">
         <v>6.0000000000000002E-5</v>
       </c>
       <c r="N6" s="4">
@@ -1239,7 +1267,7 @@
       <c r="O6" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="P6" s="26" t="s">
+      <c r="P6" s="20" t="s">
         <v>34</v>
       </c>
       <c r="Q6" s="6">
@@ -1247,16 +1275,16 @@
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A7" s="20">
+      <c r="A7" s="14">
         <v>5</v>
       </c>
-      <c r="B7" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" s="25" t="s">
+      <c r="B7" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="25" t="s">
+      <c r="D7" s="19" t="s">
         <v>32</v>
       </c>
       <c r="E7" s="2" t="s">
@@ -1265,7 +1293,7 @@
       <c r="F7" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G7" s="24" t="s">
+      <c r="G7" s="18" t="s">
         <v>31</v>
       </c>
       <c r="H7" s="3" t="s">
@@ -1280,10 +1308,10 @@
       <c r="K7" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="L7" s="24" t="s">
+      <c r="L7" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="M7" s="21">
+      <c r="M7" s="15">
         <v>6.0000000000000002E-5</v>
       </c>
       <c r="N7" s="4">
@@ -1300,16 +1328,16 @@
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A8" s="20">
+      <c r="A8" s="14">
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="23" t="s">
+      <c r="C8" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="D8" s="25" t="s">
+      <c r="D8" s="19" t="s">
         <v>32</v>
       </c>
       <c r="E8" s="2" t="s">
@@ -1318,7 +1346,7 @@
       <c r="F8" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G8" s="24" t="s">
+      <c r="G8" s="18" t="s">
         <v>31</v>
       </c>
       <c r="H8" s="3" t="s">
@@ -1333,10 +1361,10 @@
       <c r="K8" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="L8" s="24" t="s">
+      <c r="L8" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="M8" s="21">
+      <c r="M8" s="15">
         <v>5.0000000000000004E-6</v>
       </c>
       <c r="N8" s="4">
@@ -1353,16 +1381,16 @@
       </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A9" s="20">
+      <c r="A9" s="14">
         <v>7</v>
       </c>
-      <c r="B9" s="23" t="s">
+      <c r="B9" s="17" t="s">
         <v>37</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D9" s="25" t="s">
+      <c r="D9" s="19" t="s">
         <v>38</v>
       </c>
       <c r="E9" s="2" t="s">
@@ -1380,7 +1408,7 @@
       <c r="I9" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="J9" s="22" t="s">
+      <c r="J9" s="16" t="s">
         <v>45</v>
       </c>
       <c r="K9" s="3" t="s">
@@ -1389,7 +1417,7 @@
       <c r="L9" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="M9" s="21">
+      <c r="M9" s="15">
         <v>5.0000000000000004E-6</v>
       </c>
       <c r="N9" s="4">
@@ -1406,7 +1434,7 @@
       </c>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A10" s="20">
+      <c r="A10" s="14">
         <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -1415,7 +1443,7 @@
       <c r="C10" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D10" s="25" t="s">
+      <c r="D10" s="19" t="s">
         <v>42</v>
       </c>
       <c r="E10" s="2" t="s">
@@ -1442,7 +1470,7 @@
       <c r="L10" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="M10" s="21">
+      <c r="M10" s="15">
         <v>5.0000000000000004E-6</v>
       </c>
       <c r="N10" s="4">
@@ -1471,7 +1499,7 @@
       </c>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A11" s="20">
+      <c r="A11" s="14">
         <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -1480,7 +1508,7 @@
       <c r="C11" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D11" s="25" t="s">
+      <c r="D11" s="19" t="s">
         <v>42</v>
       </c>
       <c r="E11" s="2" t="s">
@@ -1495,7 +1523,7 @@
       <c r="H11" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="I11" s="22" t="s">
+      <c r="I11" s="16" t="s">
         <v>45</v>
       </c>
       <c r="J11" s="3" t="s">
@@ -1504,10 +1532,10 @@
       <c r="K11" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="L11" s="27" t="s">
+      <c r="L11" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="M11" s="21">
+      <c r="M11" s="15">
         <v>5.0000000000000004E-6</v>
       </c>
       <c r="N11" s="4">
@@ -1524,7 +1552,7 @@
       </c>
     </row>
     <row r="12" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="20">
+      <c r="A12" s="14">
         <v>10</v>
       </c>
       <c r="B12" s="2" t="s">
@@ -1533,13 +1561,13 @@
       <c r="C12" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D12" s="25" t="s">
+      <c r="D12" s="19" t="s">
         <v>42</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F12" s="23" t="s">
+      <c r="F12" s="17" t="s">
         <v>37</v>
       </c>
       <c r="G12" s="3" t="s">
@@ -1548,7 +1576,7 @@
       <c r="H12" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="I12" s="22" t="s">
+      <c r="I12" s="16" t="s">
         <v>26</v>
       </c>
       <c r="J12" s="3" t="s">
@@ -1557,10 +1585,10 @@
       <c r="K12" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="L12" s="27" t="s">
+      <c r="L12" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="M12" s="21">
+      <c r="M12" s="15">
         <v>5.0000000000000004E-6</v>
       </c>
       <c r="N12" s="4">
@@ -1577,7 +1605,7 @@
       </c>
     </row>
     <row r="13" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="20">
+      <c r="A13" s="14">
         <v>11</v>
       </c>
       <c r="B13" s="2" t="s">
@@ -1586,13 +1614,13 @@
       <c r="C13" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D13" s="25" t="s">
+      <c r="D13" s="19" t="s">
         <v>42</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F13" s="25" t="s">
+      <c r="F13" s="19" t="s">
         <v>37</v>
       </c>
       <c r="G13" s="3" t="s">
@@ -1601,7 +1629,7 @@
       <c r="H13" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="I13" s="27" t="s">
+      <c r="I13" s="21" t="s">
         <v>26</v>
       </c>
       <c r="J13" s="3" t="s">
@@ -1610,10 +1638,10 @@
       <c r="K13" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="L13" s="27" t="s">
+      <c r="L13" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="M13" s="21">
+      <c r="M13" s="15">
         <v>5.0000000000000004E-6</v>
       </c>
       <c r="N13" s="4">
@@ -1622,7 +1650,7 @@
       <c r="O13" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="P13" s="29" t="s">
+      <c r="P13" s="23" t="s">
         <v>48</v>
       </c>
       <c r="V13" s="6">
@@ -1630,7 +1658,7 @@
       </c>
     </row>
     <row r="14" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="20">
+      <c r="A14" s="14">
         <v>12</v>
       </c>
       <c r="B14" s="2" t="s">
@@ -1639,13 +1667,13 @@
       <c r="C14" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D14" s="25" t="s">
+      <c r="D14" s="19" t="s">
         <v>42</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F14" s="25" t="s">
+      <c r="F14" s="19" t="s">
         <v>37</v>
       </c>
       <c r="G14" s="3" t="s">
@@ -1654,7 +1682,7 @@
       <c r="H14" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="I14" s="27" t="s">
+      <c r="I14" s="21" t="s">
         <v>26</v>
       </c>
       <c r="J14" s="3" t="s">
@@ -1663,10 +1691,10 @@
       <c r="K14" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="L14" s="27" t="s">
+      <c r="L14" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="M14" s="21">
+      <c r="M14" s="15">
         <v>5.0000000000000004E-6</v>
       </c>
       <c r="N14" s="4">
@@ -1675,7 +1703,7 @@
       <c r="O14" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="P14" s="29" t="s">
+      <c r="P14" s="23" t="s">
         <v>49</v>
       </c>
       <c r="V14" s="6">
@@ -1683,7 +1711,7 @@
       </c>
     </row>
     <row r="15" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="20">
+      <c r="A15" s="14">
         <v>13</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -1692,13 +1720,13 @@
       <c r="C15" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D15" s="25" t="s">
+      <c r="D15" s="19" t="s">
         <v>42</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F15" s="25" t="s">
+      <c r="F15" s="19" t="s">
         <v>37</v>
       </c>
       <c r="G15" s="3" t="s">
@@ -1707,7 +1735,7 @@
       <c r="H15" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="I15" s="27" t="s">
+      <c r="I15" s="21" t="s">
         <v>26</v>
       </c>
       <c r="J15" s="3" t="s">
@@ -1716,16 +1744,16 @@
       <c r="K15" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="L15" s="27" t="s">
+      <c r="L15" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="M15" s="21">
+      <c r="M15" s="15">
         <v>5.0000000000000004E-6</v>
       </c>
       <c r="N15" s="4">
         <v>24</v>
       </c>
-      <c r="O15" s="31" t="s">
+      <c r="O15" s="25" t="s">
         <v>51</v>
       </c>
       <c r="P15" s="5" t="s">
@@ -1739,7 +1767,7 @@
       </c>
     </row>
     <row r="16" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="20">
+      <c r="A16" s="14">
         <v>14</v>
       </c>
       <c r="B16" s="2" t="s">
@@ -1748,13 +1776,13 @@
       <c r="C16" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D16" s="25" t="s">
+      <c r="D16" s="19" t="s">
         <v>42</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F16" s="25" t="s">
+      <c r="F16" s="19" t="s">
         <v>37</v>
       </c>
       <c r="G16" s="3" t="s">
@@ -1763,7 +1791,7 @@
       <c r="H16" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="I16" s="27" t="s">
+      <c r="I16" s="21" t="s">
         <v>26</v>
       </c>
       <c r="J16" s="3" t="s">
@@ -1772,19 +1800,19 @@
       <c r="K16" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="L16" s="27" t="s">
+      <c r="L16" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="M16" s="21">
+      <c r="M16" s="15">
         <v>5.0000000000000004E-6</v>
       </c>
       <c r="N16" s="4">
         <v>10</v>
       </c>
-      <c r="O16" s="32" t="s">
+      <c r="O16" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="P16" s="28" t="s">
+      <c r="P16" s="22" t="s">
         <v>50</v>
       </c>
       <c r="R16" s="6" t="s">
@@ -1795,7 +1823,7 @@
       </c>
     </row>
     <row r="17" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="20">
+      <c r="A17" s="14">
         <v>15</v>
       </c>
       <c r="B17" s="2" t="s">
@@ -1804,13 +1832,13 @@
       <c r="C17" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D17" s="25" t="s">
+      <c r="D17" s="19" t="s">
         <v>42</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F17" s="25" t="s">
+      <c r="F17" s="19" t="s">
         <v>37</v>
       </c>
       <c r="G17" s="3" t="s">
@@ -1819,7 +1847,7 @@
       <c r="H17" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="I17" s="27" t="s">
+      <c r="I17" s="21" t="s">
         <v>26</v>
       </c>
       <c r="J17" s="3" t="s">
@@ -1828,19 +1856,19 @@
       <c r="K17" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="L17" s="27" t="s">
+      <c r="L17" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="M17" s="21">
+      <c r="M17" s="15">
         <v>5.0000000000000004E-6</v>
       </c>
       <c r="N17" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="O17" s="32" t="s">
+      <c r="O17" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="P17" s="29" t="s">
+      <c r="P17" s="23" t="s">
         <v>56</v>
       </c>
       <c r="R17" s="6">
@@ -1848,7 +1876,7 @@
       </c>
     </row>
     <row r="18" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="20">
+      <c r="A18" s="14">
         <v>16</v>
       </c>
       <c r="B18" s="2" t="s">
@@ -1857,13 +1885,13 @@
       <c r="C18" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D18" s="25" t="s">
+      <c r="D18" s="19" t="s">
         <v>42</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F18" s="25" t="s">
+      <c r="F18" s="19" t="s">
         <v>37</v>
       </c>
       <c r="G18" s="3" t="s">
@@ -1872,7 +1900,7 @@
       <c r="H18" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="I18" s="27" t="s">
+      <c r="I18" s="21" t="s">
         <v>26</v>
       </c>
       <c r="J18" s="3" t="s">
@@ -1881,19 +1909,19 @@
       <c r="K18" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="L18" s="27" t="s">
+      <c r="L18" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="M18" s="21">
+      <c r="M18" s="15">
         <v>5.0000000000000004E-6</v>
       </c>
       <c r="N18" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="O18" s="32" t="s">
+      <c r="O18" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="P18" s="29" t="s">
+      <c r="P18" s="23" t="s">
         <v>57</v>
       </c>
       <c r="R18" s="6">
@@ -1901,7 +1929,7 @@
       </c>
     </row>
     <row r="19" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="20">
+      <c r="A19" s="14">
         <v>17</v>
       </c>
       <c r="B19" s="2" t="s">
@@ -1910,13 +1938,13 @@
       <c r="C19" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D19" s="25" t="s">
+      <c r="D19" s="19" t="s">
         <v>42</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F19" s="25" t="s">
+      <c r="F19" s="19" t="s">
         <v>37</v>
       </c>
       <c r="G19" s="3" t="s">
@@ -1925,7 +1953,7 @@
       <c r="H19" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="I19" s="27" t="s">
+      <c r="I19" s="21" t="s">
         <v>26</v>
       </c>
       <c r="J19" s="3" t="s">
@@ -1934,19 +1962,19 @@
       <c r="K19" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="L19" s="27" t="s">
+      <c r="L19" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="M19" s="21">
+      <c r="M19" s="15">
         <v>5.0000000000000004E-6</v>
       </c>
       <c r="N19" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="O19" s="31" t="s">
+      <c r="O19" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="P19" s="29" t="s">
+      <c r="P19" s="23" t="s">
         <v>58</v>
       </c>
       <c r="R19" s="6">
@@ -1954,7 +1982,7 @@
       </c>
     </row>
     <row r="20" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="20">
+      <c r="A20" s="14">
         <v>18</v>
       </c>
       <c r="B20" s="2" t="s">
@@ -1963,13 +1991,13 @@
       <c r="C20" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D20" s="25" t="s">
+      <c r="D20" s="19" t="s">
         <v>42</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F20" s="25" t="s">
+      <c r="F20" s="19" t="s">
         <v>37</v>
       </c>
       <c r="G20" s="3" t="s">
@@ -1978,7 +2006,7 @@
       <c r="H20" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="I20" s="27" t="s">
+      <c r="I20" s="21" t="s">
         <v>26</v>
       </c>
       <c r="J20" s="3" t="s">
@@ -1987,19 +2015,19 @@
       <c r="K20" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="L20" s="27" t="s">
+      <c r="L20" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="M20" s="21">
+      <c r="M20" s="15">
         <v>5.0000000000000004E-6</v>
       </c>
       <c r="N20" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="O20" s="31" t="s">
+      <c r="O20" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="P20" s="29" t="s">
+      <c r="P20" s="23" t="s">
         <v>59</v>
       </c>
       <c r="R20" s="6">
@@ -2007,7 +2035,7 @@
       </c>
     </row>
     <row r="21" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="20">
+      <c r="A21" s="14">
         <v>19</v>
       </c>
       <c r="B21" s="2" t="s">
@@ -2016,13 +2044,13 @@
       <c r="C21" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D21" s="25" t="s">
+      <c r="D21" s="19" t="s">
         <v>42</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F21" s="23" t="s">
+      <c r="F21" s="17" t="s">
         <v>26</v>
       </c>
       <c r="G21" s="3" t="s">
@@ -2031,7 +2059,7 @@
       <c r="H21" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="I21" s="27" t="s">
+      <c r="I21" s="21" t="s">
         <v>26</v>
       </c>
       <c r="J21" s="3" t="s">
@@ -2040,10 +2068,10 @@
       <c r="K21" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="L21" s="27" t="s">
+      <c r="L21" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="M21" s="21">
+      <c r="M21" s="15">
         <v>5.0000000000000004E-6</v>
       </c>
       <c r="N21" s="4" t="s">
@@ -2052,7 +2080,7 @@
       <c r="O21" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="P21" s="29" t="s">
+      <c r="P21" s="23" t="s">
         <v>63</v>
       </c>
       <c r="R21" s="6">
@@ -2060,7 +2088,7 @@
       </c>
     </row>
     <row r="22" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="20">
+      <c r="A22" s="36">
         <v>20</v>
       </c>
       <c r="B22" s="2" t="s">
@@ -2069,13 +2097,13 @@
       <c r="C22" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D22" s="33" t="s">
+      <c r="D22" s="27" t="s">
         <v>64</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F22" s="23" t="s">
+      <c r="F22" s="17" t="s">
         <v>37</v>
       </c>
       <c r="G22" s="3" t="s">
@@ -2084,7 +2112,7 @@
       <c r="H22" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="I22" s="27" t="s">
+      <c r="I22" s="21" t="s">
         <v>26</v>
       </c>
       <c r="J22" s="3" t="s">
@@ -2096,7 +2124,7 @@
       <c r="L22" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="M22" s="21">
+      <c r="M22" s="15">
         <v>5.0000000000000004E-6</v>
       </c>
       <c r="N22" s="4" t="s">
@@ -2105,7 +2133,7 @@
       <c r="O22" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="P22" s="29" t="s">
+      <c r="P22" s="23" t="s">
         <v>65</v>
       </c>
       <c r="V22" s="6">
@@ -2113,7 +2141,7 @@
       </c>
     </row>
     <row r="23" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="20">
+      <c r="A23" s="14">
         <v>21</v>
       </c>
       <c r="B23" s="2" t="s">
@@ -2122,13 +2150,13 @@
       <c r="C23" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D23" s="23" t="s">
+      <c r="D23" s="17" t="s">
         <v>42</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F23" s="25" t="s">
+      <c r="F23" s="19" t="s">
         <v>37</v>
       </c>
       <c r="G23" s="3" t="s">
@@ -2137,7 +2165,7 @@
       <c r="H23" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="I23" s="22" t="s">
+      <c r="I23" s="16" t="s">
         <v>45</v>
       </c>
       <c r="J23" s="3" t="s">
@@ -2149,7 +2177,7 @@
       <c r="L23" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="M23" s="21">
+      <c r="M23" s="15">
         <v>5.0000000000000004E-6</v>
       </c>
       <c r="N23" s="4" t="s">
@@ -2158,7 +2186,7 @@
       <c r="O23" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="P23" s="29" t="s">
+      <c r="P23" s="23" t="s">
         <v>66</v>
       </c>
       <c r="V23" s="6">
@@ -2166,7 +2194,7 @@
       </c>
     </row>
     <row r="24" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="20">
+      <c r="A24" s="14">
         <v>22</v>
       </c>
       <c r="B24" s="2" t="s">
@@ -2175,13 +2203,13 @@
       <c r="C24" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D24" s="33" t="s">
+      <c r="D24" s="27" t="s">
         <v>64</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F24" s="25" t="s">
+      <c r="F24" s="19" t="s">
         <v>37</v>
       </c>
       <c r="G24" s="3" t="s">
@@ -2190,7 +2218,7 @@
       <c r="H24" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="I24" s="22" t="s">
+      <c r="I24" s="16" t="s">
         <v>26</v>
       </c>
       <c r="J24" s="3" t="s">
@@ -2202,7 +2230,7 @@
       <c r="L24" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="M24" s="21">
+      <c r="M24" s="15">
         <v>5.0000000000000004E-6</v>
       </c>
       <c r="N24" s="4" t="s">
@@ -2211,7 +2239,7 @@
       <c r="O24" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="P24" s="29" t="s">
+      <c r="P24" s="23" t="s">
         <v>67</v>
       </c>
       <c r="S24" s="6">
@@ -2222,7 +2250,7 @@
       </c>
     </row>
     <row r="25" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="20">
+      <c r="A25" s="14">
         <v>23</v>
       </c>
       <c r="B25" s="2" t="s">
@@ -2231,13 +2259,13 @@
       <c r="C25" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D25" s="34" t="s">
+      <c r="D25" s="28" t="s">
         <v>64</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F25" s="25" t="s">
+      <c r="F25" s="19" t="s">
         <v>37</v>
       </c>
       <c r="G25" s="3" t="s">
@@ -2246,7 +2274,7 @@
       <c r="H25" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="I25" s="27" t="s">
+      <c r="I25" s="21" t="s">
         <v>26</v>
       </c>
       <c r="J25" s="3" t="s">
@@ -2258,7 +2286,7 @@
       <c r="L25" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="M25" s="21">
+      <c r="M25" s="15">
         <v>5.0000000000000004E-6</v>
       </c>
       <c r="N25" s="4" t="s">
@@ -2267,7 +2295,7 @@
       <c r="O25" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="P25" s="29" t="s">
+      <c r="P25" s="23" t="s">
         <v>68</v>
       </c>
       <c r="V25" s="6">
@@ -2275,7 +2303,7 @@
       </c>
     </row>
     <row r="26" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="20">
+      <c r="A26" s="14">
         <v>24</v>
       </c>
       <c r="B26" s="2" t="s">
@@ -2284,7 +2312,7 @@
       <c r="C26" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D26" s="23" t="s">
+      <c r="D26" s="17" t="s">
         <v>42</v>
       </c>
       <c r="E26" s="2" t="s">
@@ -2299,23 +2327,23 @@
       <c r="H26" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="I26" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="J26" s="22" t="s">
-        <v>71</v>
+      <c r="I26" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="J26" s="16" t="s">
+        <v>82</v>
       </c>
       <c r="K26" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="L26" s="22" t="s">
-        <v>70</v>
-      </c>
-      <c r="M26" s="21">
+      <c r="L26" s="39" t="s">
+        <v>78</v>
+      </c>
+      <c r="M26" s="15">
         <v>5.0000000000000004E-6</v>
       </c>
-      <c r="N26" s="30" t="s">
-        <v>70</v>
+      <c r="N26" s="38">
+        <v>17</v>
       </c>
       <c r="O26" s="4" t="s">
         <v>26</v>
@@ -2323,12 +2351,12 @@
       <c r="P26" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="V26" s="35" t="s">
-        <v>70</v>
+      <c r="V26" s="37">
+        <v>0.56999999999999995</v>
       </c>
     </row>
     <row r="27" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="20">
+      <c r="A27" s="14">
         <v>25</v>
       </c>
       <c r="B27" s="2" t="s">
@@ -2337,7 +2365,7 @@
       <c r="C27" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D27" s="33" t="s">
+      <c r="D27" s="27" t="s">
         <v>64</v>
       </c>
       <c r="E27" s="2" t="s">
@@ -2352,7 +2380,7 @@
       <c r="H27" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="I27" s="27" t="s">
+      <c r="I27" s="21" t="s">
         <v>26</v>
       </c>
       <c r="J27" s="3" t="s">
@@ -2364,11 +2392,11 @@
       <c r="L27" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="M27" s="21">
+      <c r="M27" s="15">
         <v>5.0000000000000004E-6</v>
       </c>
-      <c r="N27" s="30" t="s">
-        <v>70</v>
+      <c r="N27" s="38">
+        <v>29</v>
       </c>
       <c r="O27" s="4" t="s">
         <v>26</v>
@@ -2376,12 +2404,12 @@
       <c r="P27" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="V27" s="35" t="s">
-        <v>70</v>
+      <c r="V27" s="37">
+        <v>0.6</v>
       </c>
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A28" s="20">
+      <c r="A28" s="14">
         <v>26</v>
       </c>
       <c r="B28" s="2" t="s">
@@ -2390,7 +2418,7 @@
       <c r="C28" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D28" s="23" t="s">
+      <c r="D28" s="17" t="s">
         <v>42</v>
       </c>
       <c r="E28" s="2" t="s">
@@ -2405,23 +2433,23 @@
       <c r="H28" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="I28" s="27" t="s">
+      <c r="I28" s="21" t="s">
         <v>26</v>
       </c>
       <c r="J28" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="K28" s="22" t="s">
+      <c r="K28" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="L28" s="22" t="s">
-        <v>70</v>
-      </c>
-      <c r="M28" s="21">
+      <c r="L28" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="M28" s="15">
         <v>5.0000000000000004E-6</v>
       </c>
-      <c r="N28" s="30" t="s">
-        <v>70</v>
+      <c r="N28" s="38">
+        <v>12</v>
       </c>
       <c r="O28" s="4" t="s">
         <v>26</v>
@@ -2429,12 +2457,12 @@
       <c r="P28" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="V28" s="35" t="s">
-        <v>70</v>
+      <c r="V28" s="37">
+        <v>0.53</v>
       </c>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A29" s="20">
+      <c r="A29" s="14">
         <v>27</v>
       </c>
       <c r="B29" s="2" t="s">
@@ -2443,7 +2471,7 @@
       <c r="C29" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D29" s="25" t="s">
+      <c r="D29" s="19" t="s">
         <v>42</v>
       </c>
       <c r="E29" s="2" t="s">
@@ -2458,23 +2486,23 @@
       <c r="H29" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="I29" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="J29" s="22" t="s">
+      <c r="I29" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="J29" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="K29" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="K29" s="27" t="s">
-        <v>71</v>
-      </c>
-      <c r="L29" s="22" t="s">
-        <v>70</v>
-      </c>
-      <c r="M29" s="21">
+      <c r="L29" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="M29" s="15">
         <v>5.0000000000000004E-6</v>
       </c>
-      <c r="N29" s="30" t="s">
-        <v>70</v>
+      <c r="N29" s="38">
+        <v>10</v>
       </c>
       <c r="O29" s="4" t="s">
         <v>26</v>
@@ -2482,12 +2510,12 @@
       <c r="P29" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="V29" s="35" t="s">
-        <v>70</v>
+      <c r="V29" s="37">
+        <v>0.53</v>
       </c>
     </row>
     <row r="30" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A30" s="20">
+      <c r="A30" s="14">
         <v>28</v>
       </c>
       <c r="B30" s="2" t="s">
@@ -2496,13 +2524,13 @@
       <c r="C30" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D30" s="25" t="s">
+      <c r="D30" s="19" t="s">
         <v>42</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F30" s="23" t="s">
+      <c r="F30" s="17" t="s">
         <v>26</v>
       </c>
       <c r="G30" s="3" t="s">
@@ -2511,23 +2539,23 @@
       <c r="H30" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="I30" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="J30" s="27" t="s">
+      <c r="I30" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="J30" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="K30" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="K30" s="27" t="s">
-        <v>71</v>
-      </c>
-      <c r="L30" s="22" t="s">
-        <v>70</v>
-      </c>
-      <c r="M30" s="21">
+      <c r="L30" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="M30" s="15">
         <v>5.0000000000000004E-6</v>
       </c>
-      <c r="N30" s="30" t="s">
-        <v>70</v>
+      <c r="N30" s="38">
+        <v>12</v>
       </c>
       <c r="O30" s="4" t="s">
         <v>26</v>
@@ -2535,12 +2563,12 @@
       <c r="P30" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="V30" s="35" t="s">
-        <v>70</v>
+      <c r="V30" s="37">
+        <v>0.51</v>
       </c>
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A31" s="20">
+      <c r="A31" s="14">
         <v>29</v>
       </c>
       <c r="B31" s="2" t="s">
@@ -2549,15 +2577,48 @@
       <c r="C31" s="2" t="s">
         <v>36</v>
       </c>
+      <c r="D31" s="19" t="s">
+        <v>42</v>
+      </c>
       <c r="E31" s="2" t="s">
         <v>26</v>
       </c>
+      <c r="F31" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H31" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I31" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="J31" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="K31" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="L31" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="N31" s="24" t="s">
+        <v>70</v>
+      </c>
       <c r="O31" s="4" t="s">
         <v>26</v>
       </c>
+      <c r="P31" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="V31" s="29" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="32" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A32" s="20">
+      <c r="A32" s="14">
         <v>30</v>
       </c>
       <c r="B32" s="2" t="s">
@@ -2566,15 +2627,48 @@
       <c r="C32" s="2" t="s">
         <v>36</v>
       </c>
+      <c r="D32" s="19" t="s">
+        <v>42</v>
+      </c>
       <c r="E32" s="2" t="s">
         <v>26</v>
       </c>
+      <c r="F32" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H32" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I32" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="J32" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="K32" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="L32" s="39" t="s">
+        <v>78</v>
+      </c>
+      <c r="N32" s="24" t="s">
+        <v>70</v>
+      </c>
       <c r="O32" s="4" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A33" s="20">
+      <c r="P32" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="V32" s="29" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="33" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A33" s="14">
         <v>31</v>
       </c>
       <c r="B33" s="2" t="s">
@@ -2583,95 +2677,72 @@
       <c r="C33" s="2" t="s">
         <v>36</v>
       </c>
+      <c r="D33" s="19" t="s">
+        <v>42</v>
+      </c>
       <c r="E33" s="2" t="s">
         <v>26</v>
       </c>
+      <c r="F33" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H33" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I33" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="J33" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="K33" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="L33" s="39"/>
+      <c r="N33" s="24" t="s">
+        <v>70</v>
+      </c>
       <c r="O33" s="4" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A34" s="20">
+      <c r="P33" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="V33" s="29" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="34" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A34" s="14">
         <v>32</v>
       </c>
-      <c r="B34" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C34" s="2" t="s">
+    </row>
+    <row r="35" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A35" s="14">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A36" s="14">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="37" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A37" s="14">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="38" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A38" s="14">
         <v>36</v>
       </c>
-      <c r="E34" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A35" s="20">
-        <v>33</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A36" s="20">
-        <v>34</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A37" s="20">
-        <v>35</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A38" s="20">
-        <v>36</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A39" s="20">
-        <v>37</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>26</v>
+    </row>
+    <row r="39" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A39" s="14">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -2684,14 +2755,6 @@
     <mergeCell ref="M1:O1"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
-  <conditionalFormatting sqref="B1:F2">
-    <cfRule type="expression" dxfId="1" priority="1">
-      <formula>'TRUE'</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="0" priority="2">
-      <formula>'TRUE'</formula>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>